<commit_message>
Added course scheduling feature to project.
</commit_message>
<xml_diff>
--- a/GACourseAndExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
+++ b/GACourseAndExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcht6\source\repos\GAExamSchedule\GAExamSchedule\ScheduleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcht6\source\repos\GACourseAndExamSchedule\GACourseAndExamSchedule\ScheduleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80EEEBE-02B0-4B1B-AAE5-B9D3EF7476F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D9F1C6-38DB-481D-BFB4-88102570132A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
   <si>
     <t>Öğrenci Sayısı</t>
   </si>
@@ -110,13 +107,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01E95F90-8495-4C20-B6D7-669D33C6CB28}" name="Tablo1" displayName="Tablo1" ref="A1:I29" totalsRowShown="0">
-  <autoFilter ref="A1:I29" xr:uid="{97CFA720-D15B-4545-9496-9AAF040BF23F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
-    <sortCondition ref="A1:A17"/>
-  </sortState>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{BA756C68-461A-4DE7-8F9B-C5D17F55712D}" name="ID"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01E95F90-8495-4C20-B6D7-669D33C6CB28}" name="Tablo1" displayName="Tablo1" ref="A1:H29" totalsRowShown="0">
+  <autoFilter ref="A1:H29" xr:uid="{97CFA720-D15B-4545-9496-9AAF040BF23F}"/>
+  <tableColumns count="8">
     <tableColumn id="2" xr3:uid="{F92667C9-B76B-4CC8-A151-8A07A1483D51}" name="Ders"/>
     <tableColumn id="3" xr3:uid="{4E99577D-0171-40E1-83D8-AC4C0E25D1CA}" name="Öğretim Görevlisi"/>
     <tableColumn id="4" xr3:uid="{CF1CBA5F-007E-48CD-922B-3B6F9EEFDB6D}" name="Süre"/>
@@ -393,25 +386,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -426,19 +419,16 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -446,144 +436,129 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
       </c>
       <c r="G2">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
       </c>
       <c r="G3">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
       </c>
       <c r="G5">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -591,662 +566,593 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
       </c>
       <c r="G7">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
       </c>
       <c r="G8">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
       </c>
       <c r="G9">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
       </c>
       <c r="G10">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
-        <v>7</v>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
-        <v>7</v>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
       </c>
       <c r="G12">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
-        <v>7</v>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
       </c>
       <c r="G13">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
-        <v>7</v>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>40</v>
       </c>
       <c r="G14">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
         <v>4</v>
       </c>
-      <c r="F15" t="s">
-        <v>7</v>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
       </c>
       <c r="G15">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
         <v>4</v>
       </c>
-      <c r="F16" t="s">
-        <v>7</v>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
       </c>
       <c r="G16">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
         <v>4</v>
       </c>
-      <c r="F17" t="s">
-        <v>7</v>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>40</v>
       </c>
       <c r="G17">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
         <v>5</v>
       </c>
-      <c r="F18" t="s">
-        <v>7</v>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>40</v>
       </c>
       <c r="G18">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C19">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
         <v>5</v>
       </c>
-      <c r="F19" t="s">
-        <v>7</v>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>40</v>
       </c>
       <c r="G19">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>40</v>
       </c>
       <c r="G20">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>40</v>
       </c>
       <c r="G21">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>6</v>
-      </c>
-      <c r="F22" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>40</v>
       </c>
       <c r="G22">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
         <v>7</v>
       </c>
-      <c r="F23" t="s">
-        <v>7</v>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23">
+        <v>40</v>
       </c>
       <c r="G23">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
         <v>7</v>
       </c>
-      <c r="F24" t="s">
-        <v>7</v>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>40</v>
       </c>
       <c r="G24">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="H24">
-        <v>3</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25">
         <v>7</v>
       </c>
-      <c r="F25" t="s">
-        <v>7</v>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>40</v>
       </c>
       <c r="G25">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
         <v>8</v>
       </c>
-      <c r="F26" t="s">
-        <v>7</v>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>40</v>
       </c>
       <c r="G26">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="H26">
-        <v>3</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="E27">
         <v>8</v>
       </c>
-      <c r="F27" t="s">
-        <v>7</v>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>40</v>
       </c>
       <c r="G27">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>2</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28">
         <v>8</v>
       </c>
-      <c r="F28" t="s">
-        <v>7</v>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <v>40</v>
       </c>
       <c r="G28">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="H28">
-        <v>3</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="E29">
         <v>8</v>
       </c>
-      <c r="F29" t="s">
-        <v>7</v>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <v>40</v>
       </c>
       <c r="G29">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="H29">
-        <v>2</v>
-      </c>
-      <c r="I29">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed calculate fitness functions.
</commit_message>
<xml_diff>
--- a/GACourseAndExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
+++ b/GACourseAndExamSchedule/ScheduleData/Ders Eşleştirmeleri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcht6\source\repos\GACourseAndExamSchedule\GACourseAndExamSchedule\ScheduleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D9F1C6-38DB-481D-BFB4-88102570132A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F40795-F8C4-4A6A-8BAB-04C463E0AC2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
-  <si>
-    <t>Öğrenci Sayısı</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
   <si>
     <t>Ders</t>
   </si>
   <si>
     <t>Öğretim Görevlisi</t>
-  </si>
-  <si>
-    <t>Süre</t>
   </si>
   <si>
     <t>Öğrenci Grupları</t>
@@ -52,6 +46,15 @@
   </si>
   <si>
     <t>Sınıf Sayısı</t>
+  </si>
+  <si>
+    <t>Ders Süresi</t>
+  </si>
+  <si>
+    <t>Sınav Süresi</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -107,15 +110,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01E95F90-8495-4C20-B6D7-669D33C6CB28}" name="Tablo1" displayName="Tablo1" ref="A1:H29" totalsRowShown="0">
-  <autoFilter ref="A1:H29" xr:uid="{97CFA720-D15B-4545-9496-9AAF040BF23F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{01E95F90-8495-4C20-B6D7-669D33C6CB28}" name="Tablo1" displayName="Tablo1" ref="A1:H33" totalsRowShown="0">
+  <autoFilter ref="A1:H33" xr:uid="{97CFA720-D15B-4545-9496-9AAF040BF23F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H28">
+    <sortCondition ref="B1:B28"/>
+  </sortState>
   <tableColumns count="8">
     <tableColumn id="2" xr3:uid="{F92667C9-B76B-4CC8-A151-8A07A1483D51}" name="Ders"/>
     <tableColumn id="3" xr3:uid="{4E99577D-0171-40E1-83D8-AC4C0E25D1CA}" name="Öğretim Görevlisi"/>
-    <tableColumn id="4" xr3:uid="{CF1CBA5F-007E-48CD-922B-3B6F9EEFDB6D}" name="Süre"/>
+    <tableColumn id="1" xr3:uid="{C947BE5B-9FC8-4195-A78D-56856325BDEC}" name="Ders Süresi"/>
+    <tableColumn id="4" xr3:uid="{CF1CBA5F-007E-48CD-922B-3B6F9EEFDB6D}" name="Sınav Süresi"/>
     <tableColumn id="5" xr3:uid="{1181698C-0040-42DA-B8A8-38E64FBA0A8B}" name="Öğrenci Grupları"/>
     <tableColumn id="6" xr3:uid="{CD6186F9-608C-41C9-93CC-741E77862B4F}" name="Laboratuvar Gereksinimi (E - H)"/>
-    <tableColumn id="7" xr3:uid="{1B634FA2-8C2F-40A9-B561-63620074B0D4}" name="Öğrenci Sayısı"/>
     <tableColumn id="8" xr3:uid="{6FCE4EE1-7A26-4B09-89C4-5BD6B2EE2368}" name="Zorluk"/>
     <tableColumn id="9" xr3:uid="{04857D93-366D-4A91-9EC7-7235D31969AE}" name="Sınıf Sayısı"/>
   </tableColumns>
@@ -386,46 +392,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -433,25 +440,25 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -459,25 +466,25 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -488,22 +495,22 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -514,22 +521,22 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1.5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -537,25 +544,25 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>40</v>
+      <c r="E6">
+        <v>2.6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -563,25 +570,25 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>40</v>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -589,25 +596,25 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>40</v>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -615,25 +622,25 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>40</v>
+      <c r="E9">
+        <v>2.6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -641,25 +648,25 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10">
-        <v>40</v>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -667,25 +674,25 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -693,25 +700,25 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -722,22 +729,22 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -745,25 +752,25 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>4</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -771,25 +778,25 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -797,25 +804,25 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -823,25 +830,25 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -849,25 +856,25 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -875,25 +882,25 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -901,25 +908,25 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>4</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -927,25 +934,25 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
         <v>6</v>
       </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21">
-        <v>40</v>
+      <c r="F21" t="s">
+        <v>4</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -953,25 +960,25 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
         <v>6</v>
       </c>
-      <c r="E22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22">
-        <v>40</v>
+      <c r="F22" t="s">
+        <v>4</v>
       </c>
       <c r="G22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -979,25 +986,25 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23">
         <v>6</v>
       </c>
-      <c r="F23">
-        <v>40</v>
+      <c r="F23" t="s">
+        <v>4</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1005,25 +1012,25 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
         <v>7</v>
       </c>
-      <c r="E24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24">
-        <v>40</v>
+      <c r="F24" t="s">
+        <v>4</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1031,25 +1038,25 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
         <v>7</v>
       </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25">
-        <v>40</v>
+      <c r="F25" t="s">
+        <v>4</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1057,25 +1064,25 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1083,25 +1090,25 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>4</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1109,25 +1116,25 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1135,25 +1142,129 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
         <v>8</v>
       </c>
-      <c r="E29" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29">
-        <v>40</v>
+      <c r="F29" t="s">
+        <v>4</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>8</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>